<commit_message>
miscelleneous file to condense different spreadsheet
</commit_message>
<xml_diff>
--- a/planning/greenhouse_design/greenhousedesign.xlsx
+++ b/planning/greenhouse_design/greenhousedesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/planning/greenhouse_design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA05DDF6-5EE4-4846-911F-08BDADFFBD79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22712A46-0E81-D64D-A5AF-658715A53F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{D6621B14-A242-0E4C-80F5-D7CC9E637369}"/>
   </bookViews>
@@ -111,7 +111,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,12 +175,6 @@
       <sz val="7"/>
       <color theme="1"/>
       <name val="Helvetica"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -442,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -570,50 +564,49 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -962,153 +955,153 @@
   </sheetPr>
   <dimension ref="A1:BB45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="284" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="93" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" style="59"/>
-    <col min="2" max="2" width="2.6640625" style="59" customWidth="1"/>
-    <col min="3" max="3" width="5.83203125" style="59"/>
-    <col min="4" max="4" width="2.33203125" style="60" customWidth="1"/>
-    <col min="5" max="5" width="5.83203125" style="59"/>
-    <col min="6" max="6" width="2.6640625" style="59" customWidth="1"/>
-    <col min="7" max="7" width="5.83203125" style="59"/>
-    <col min="8" max="8" width="2" style="59" customWidth="1"/>
-    <col min="9" max="9" width="5.83203125" style="59"/>
-    <col min="10" max="10" width="2.6640625" style="59" customWidth="1"/>
-    <col min="11" max="11" width="5.83203125" style="59"/>
-    <col min="12" max="12" width="2" style="59" customWidth="1"/>
-    <col min="13" max="13" width="5.83203125" style="59"/>
-    <col min="14" max="14" width="2.6640625" style="59" customWidth="1"/>
-    <col min="15" max="15" width="5.83203125" style="59"/>
-    <col min="16" max="16" width="2" style="59" customWidth="1"/>
-    <col min="17" max="17" width="5.83203125" style="59"/>
-    <col min="18" max="18" width="2.6640625" style="59" customWidth="1"/>
-    <col min="19" max="19" width="5.83203125" style="59"/>
-    <col min="20" max="20" width="2" style="59" customWidth="1"/>
-    <col min="21" max="21" width="5.83203125" style="59"/>
-    <col min="22" max="22" width="2.6640625" style="59" customWidth="1"/>
-    <col min="23" max="23" width="5.83203125" style="59"/>
-    <col min="24" max="24" width="2" style="59" customWidth="1"/>
-    <col min="25" max="25" width="5.83203125" style="59"/>
-    <col min="26" max="26" width="2.6640625" style="59" customWidth="1"/>
-    <col min="27" max="27" width="5.83203125" style="59"/>
-    <col min="28" max="28" width="2.6640625" style="59" customWidth="1"/>
-    <col min="29" max="29" width="5.83203125" style="59"/>
-    <col min="30" max="30" width="2.6640625" style="59" customWidth="1"/>
-    <col min="31" max="31" width="5.83203125" style="59"/>
-    <col min="32" max="32" width="2" style="59" customWidth="1"/>
-    <col min="33" max="33" width="5.83203125" style="59"/>
-    <col min="34" max="34" width="2.6640625" style="59" customWidth="1"/>
-    <col min="35" max="35" width="5.83203125" style="59"/>
-    <col min="36" max="36" width="2" style="59" customWidth="1"/>
-    <col min="37" max="37" width="5.83203125" style="59"/>
-    <col min="38" max="38" width="2.6640625" style="59" customWidth="1"/>
-    <col min="39" max="39" width="5.83203125" style="59"/>
-    <col min="40" max="40" width="2" style="59" customWidth="1"/>
-    <col min="41" max="41" width="5.83203125" style="59"/>
-    <col min="42" max="42" width="2.6640625" style="59" customWidth="1"/>
-    <col min="43" max="44" width="5.83203125" style="59"/>
-    <col min="45" max="45" width="13.6640625" style="59" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10" style="59" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="13" style="59" bestFit="1" customWidth="1"/>
-    <col min="48" max="16384" width="5.83203125" style="59"/>
+    <col min="1" max="1" width="5.83203125" style="1"/>
+    <col min="2" max="2" width="2.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.83203125" style="1"/>
+    <col min="4" max="4" width="2.33203125" style="49" customWidth="1"/>
+    <col min="5" max="5" width="5.83203125" style="1"/>
+    <col min="6" max="6" width="2.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" style="1"/>
+    <col min="8" max="8" width="2" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.83203125" style="1"/>
+    <col min="10" max="10" width="2.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.83203125" style="1"/>
+    <col min="12" max="12" width="2" style="1" customWidth="1"/>
+    <col min="13" max="13" width="5.83203125" style="1"/>
+    <col min="14" max="14" width="2.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="5.83203125" style="1"/>
+    <col min="16" max="16" width="2" style="1" customWidth="1"/>
+    <col min="17" max="17" width="5.83203125" style="1"/>
+    <col min="18" max="18" width="2.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="5.83203125" style="1"/>
+    <col min="20" max="20" width="2" style="1" customWidth="1"/>
+    <col min="21" max="21" width="5.83203125" style="1"/>
+    <col min="22" max="22" width="2.6640625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="5.83203125" style="1"/>
+    <col min="24" max="24" width="2" style="1" customWidth="1"/>
+    <col min="25" max="25" width="5.83203125" style="1"/>
+    <col min="26" max="26" width="2.6640625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="5.83203125" style="1"/>
+    <col min="28" max="28" width="2.6640625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="5.83203125" style="1"/>
+    <col min="30" max="30" width="2.6640625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="5.83203125" style="1"/>
+    <col min="32" max="32" width="2" style="1" customWidth="1"/>
+    <col min="33" max="33" width="5.83203125" style="1"/>
+    <col min="34" max="34" width="2.6640625" style="1" customWidth="1"/>
+    <col min="35" max="35" width="5.83203125" style="1"/>
+    <col min="36" max="36" width="2" style="1" customWidth="1"/>
+    <col min="37" max="37" width="5.83203125" style="1"/>
+    <col min="38" max="38" width="2.6640625" style="1" customWidth="1"/>
+    <col min="39" max="39" width="5.83203125" style="1"/>
+    <col min="40" max="40" width="2" style="1" customWidth="1"/>
+    <col min="41" max="41" width="5.83203125" style="1"/>
+    <col min="42" max="42" width="2.6640625" style="1" customWidth="1"/>
+    <col min="43" max="44" width="5.83203125" style="1"/>
+    <col min="45" max="45" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="16384" width="5.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="53" t="s">
+      <c r="A1" s="57"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
+      <c r="U1" s="57"/>
+      <c r="V1" s="57"/>
+      <c r="W1" s="57"/>
+      <c r="X1" s="57"/>
+      <c r="Y1" s="57"/>
+      <c r="Z1" s="57"/>
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="AD1" s="50"/>
-      <c r="AE1" s="50"/>
-      <c r="AF1" s="50"/>
-      <c r="AG1" s="50"/>
-      <c r="AH1" s="50"/>
-      <c r="AI1" s="50"/>
-      <c r="AJ1" s="50"/>
-      <c r="AK1" s="50"/>
-      <c r="AL1" s="50"/>
-      <c r="AM1" s="50"/>
-      <c r="AN1" s="50"/>
-      <c r="AO1" s="50"/>
-      <c r="AP1" s="50"/>
+      <c r="AD1" s="57"/>
+      <c r="AE1" s="57"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="57"/>
+      <c r="AJ1" s="57"/>
+      <c r="AK1" s="57"/>
+      <c r="AL1" s="57"/>
+      <c r="AM1" s="57"/>
+      <c r="AN1" s="57"/>
+      <c r="AO1" s="57"/>
+      <c r="AP1" s="57"/>
       <c r="AQ1" s="2"/>
     </row>
     <row r="2" spans="1:54" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="48"/>
-      <c r="AB2" s="55"/>
-      <c r="AC2" s="47" t="s">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="AD2" s="48"/>
-      <c r="AE2" s="48"/>
-      <c r="AF2" s="48"/>
-      <c r="AG2" s="48"/>
-      <c r="AH2" s="48"/>
-      <c r="AI2" s="48"/>
-      <c r="AJ2" s="48"/>
-      <c r="AK2" s="48"/>
-      <c r="AL2" s="48"/>
-      <c r="AM2" s="48"/>
-      <c r="AN2" s="48"/>
-      <c r="AO2" s="48"/>
-      <c r="AP2" s="48"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
+      <c r="AF2" s="54"/>
+      <c r="AG2" s="54"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
+      <c r="AL2" s="54"/>
+      <c r="AM2" s="54"/>
+      <c r="AN2" s="54"/>
+      <c r="AO2" s="54"/>
+      <c r="AP2" s="54"/>
       <c r="AQ2" s="12"/>
     </row>
     <row r="3" spans="1:54" s="8" customFormat="1" ht="76" customHeight="1" x14ac:dyDescent="0.2">
@@ -1204,11 +1197,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="32"/>
       <c r="C4" s="4"/>
-      <c r="D4" s="57">
+      <c r="D4" s="47">
         <v>5486</v>
       </c>
       <c r="E4" s="4"/>
@@ -1218,18 +1211,18 @@
       <c r="I4" s="4"/>
       <c r="J4" s="32"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="57">
+      <c r="L4" s="47">
         <v>5912</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="32"/>
-      <c r="O4" s="64">
+      <c r="O4" s="52">
         <v>8424</v>
       </c>
-      <c r="P4" s="57">
+      <c r="P4" s="47">
         <v>5908</v>
       </c>
-      <c r="Q4" s="64">
+      <c r="Q4" s="52">
         <v>9908</v>
       </c>
       <c r="R4" s="32"/>
@@ -1238,13 +1231,13 @@
       <c r="U4" s="6"/>
       <c r="V4" s="32"/>
       <c r="W4" s="6"/>
-      <c r="X4" s="57">
+      <c r="X4" s="47">
         <v>5484</v>
       </c>
       <c r="Y4" s="6"/>
       <c r="Z4" s="32"/>
       <c r="AA4" s="6"/>
-      <c r="AB4" s="57">
+      <c r="AB4" s="47">
         <v>5493</v>
       </c>
       <c r="AC4" s="7"/>
@@ -1258,12 +1251,12 @@
       <c r="AK4" s="7"/>
       <c r="AL4" s="32"/>
       <c r="AM4" s="7"/>
-      <c r="AN4" s="57">
+      <c r="AN4" s="47">
         <v>5910</v>
       </c>
       <c r="AO4" s="7"/>
       <c r="AP4" s="5"/>
-      <c r="AR4" s="62">
+      <c r="AR4" s="50">
         <v>5931</v>
       </c>
       <c r="BA4" s="10"/>
@@ -1271,7 +1264,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:54" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="32"/>
       <c r="C5" s="4"/>
@@ -1317,7 +1310,7 @@
       <c r="AO5" s="7"/>
       <c r="AP5" s="5"/>
     </row>
-    <row r="6" spans="1:54" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="32"/>
       <c r="C6" s="4"/>
@@ -1354,7 +1347,7 @@
       <c r="AH6" s="33"/>
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
-      <c r="AK6" s="64">
+      <c r="AK6" s="52">
         <v>8485</v>
       </c>
       <c r="AL6" s="32"/>
@@ -1362,12 +1355,12 @@
       <c r="AN6" s="7"/>
       <c r="AO6" s="7"/>
       <c r="AP6" s="5"/>
-      <c r="BA6" s="58"/>
+      <c r="BA6" s="48"/>
       <c r="BB6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:54" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="32"/>
       <c r="C7" s="4"/>
@@ -1410,12 +1403,12 @@
       <c r="AN7" s="7"/>
       <c r="AO7" s="7"/>
       <c r="AP7" s="5"/>
-      <c r="BA7" s="63"/>
+      <c r="BA7" s="51"/>
       <c r="BB7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:54" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="32"/>
       <c r="C8" s="4"/>
@@ -1459,7 +1452,7 @@
       <c r="AO8" s="7"/>
       <c r="AP8" s="5"/>
     </row>
-    <row r="9" spans="1:54" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="21"/>
       <c r="B9" s="32"/>
       <c r="C9" s="21"/>
@@ -1503,7 +1496,7 @@
       <c r="AO9" s="6"/>
       <c r="AP9" s="5"/>
     </row>
-    <row r="10" spans="1:54" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="21"/>
       <c r="B10" s="32"/>
       <c r="C10" s="21"/>
@@ -1547,7 +1540,7 @@
       <c r="AO10" s="6"/>
       <c r="AP10" s="5"/>
     </row>
-    <row r="11" spans="1:54" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="21"/>
       <c r="B11" s="32"/>
       <c r="C11" s="21"/>
@@ -1591,7 +1584,7 @@
       <c r="AO11" s="6"/>
       <c r="AP11" s="5"/>
     </row>
-    <row r="12" spans="1:54" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="21"/>
       <c r="B12" s="32"/>
       <c r="C12" s="21"/>
@@ -1634,11 +1627,11 @@
       <c r="AN12" s="6"/>
       <c r="AO12" s="6"/>
       <c r="AP12" s="5"/>
-      <c r="AR12" s="62">
+      <c r="AR12" s="50">
         <v>5924</v>
       </c>
     </row>
-    <row r="13" spans="1:54" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="21"/>
       <c r="B13" s="32"/>
       <c r="C13" s="21"/>
@@ -1682,7 +1675,7 @@
       <c r="AO13" s="6"/>
       <c r="AP13" s="5"/>
     </row>
-    <row r="14" spans="1:54" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
       <c r="B14" s="32"/>
       <c r="C14" s="27"/>
@@ -1726,7 +1719,7 @@
       <c r="AO14" s="21"/>
       <c r="AP14" s="5"/>
     </row>
-    <row r="15" spans="1:54" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="27"/>
       <c r="B15" s="32"/>
       <c r="C15" s="27"/>
@@ -1770,12 +1763,12 @@
       <c r="AO15" s="21"/>
       <c r="AP15" s="5"/>
     </row>
-    <row r="16" spans="1:54" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:54" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="27"/>
       <c r="B16" s="32"/>
       <c r="C16" s="27"/>
       <c r="D16" s="43"/>
-      <c r="E16" s="64">
+      <c r="E16" s="52">
         <v>6899</v>
       </c>
       <c r="F16" s="32"/>
@@ -1816,7 +1809,7 @@
       <c r="AO16" s="21"/>
       <c r="AP16" s="5"/>
     </row>
-    <row r="17" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="27"/>
       <c r="B17" s="32"/>
       <c r="C17" s="27"/>
@@ -1860,7 +1853,7 @@
       <c r="AO17" s="21"/>
       <c r="AP17" s="5"/>
     </row>
-    <row r="18" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="27"/>
       <c r="B18" s="32"/>
       <c r="C18" s="27"/>
@@ -1904,7 +1897,7 @@
       <c r="AO18" s="21"/>
       <c r="AP18" s="5"/>
     </row>
-    <row r="19" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28"/>
       <c r="B19" s="32"/>
       <c r="C19" s="28"/>
@@ -1948,7 +1941,7 @@
       <c r="AO19" s="28"/>
       <c r="AP19" s="5"/>
     </row>
-    <row r="20" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="28"/>
       <c r="B20" s="32"/>
       <c r="C20" s="28"/>
@@ -1992,11 +1985,11 @@
       <c r="AO20" s="28"/>
       <c r="AP20" s="5"/>
     </row>
-    <row r="21" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="28"/>
       <c r="B21" s="32"/>
       <c r="C21" s="28"/>
-      <c r="D21" s="57">
+      <c r="D21" s="47">
         <v>5360</v>
       </c>
       <c r="E21" s="28"/>
@@ -2006,13 +1999,13 @@
       <c r="I21" s="28"/>
       <c r="J21" s="32"/>
       <c r="K21" s="28"/>
-      <c r="L21" s="57">
+      <c r="L21" s="47">
         <v>5358</v>
       </c>
       <c r="M21" s="28"/>
       <c r="N21" s="32"/>
       <c r="O21" s="27"/>
-      <c r="P21" s="57">
+      <c r="P21" s="47">
         <v>5916</v>
       </c>
       <c r="Q21" s="27"/>
@@ -2022,13 +2015,13 @@
       <c r="U21" s="27"/>
       <c r="V21" s="32"/>
       <c r="W21" s="27"/>
-      <c r="X21" s="57">
+      <c r="X21" s="47">
         <v>5930</v>
       </c>
       <c r="Y21" s="27"/>
       <c r="Z21" s="32"/>
       <c r="AA21" s="27"/>
-      <c r="AB21" s="57">
+      <c r="AB21" s="47">
         <v>6530</v>
       </c>
       <c r="AC21" s="28"/>
@@ -2042,16 +2035,16 @@
       <c r="AK21" s="28"/>
       <c r="AL21" s="32"/>
       <c r="AM21" s="28"/>
-      <c r="AN21" s="57">
+      <c r="AN21" s="47">
         <v>5926</v>
       </c>
       <c r="AO21" s="28"/>
       <c r="AP21" s="5"/>
-      <c r="AR21" s="62">
+      <c r="AR21" s="50">
         <v>5485</v>
       </c>
     </row>
-    <row r="22" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="28"/>
       <c r="B22" s="32"/>
       <c r="C22" s="28"/>
@@ -2095,7 +2088,7 @@
       <c r="AO22" s="28"/>
       <c r="AP22" s="5"/>
     </row>
-    <row r="23" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="28"/>
       <c r="B23" s="32"/>
       <c r="C23" s="28"/>
@@ -2139,7 +2132,7 @@
       <c r="AO23" s="28"/>
       <c r="AP23" s="5"/>
     </row>
-    <row r="24" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="32"/>
       <c r="C24" s="7"/>
@@ -2183,7 +2176,7 @@
       <c r="AO24" s="4"/>
       <c r="AP24" s="5"/>
     </row>
-    <row r="25" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="32"/>
       <c r="C25" s="7"/>
@@ -2227,7 +2220,7 @@
       <c r="AO25" s="4"/>
       <c r="AP25" s="5"/>
     </row>
-    <row r="26" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="32"/>
       <c r="C26" s="7"/>
@@ -2248,7 +2241,7 @@
       <c r="R26" s="32"/>
       <c r="S26" s="21"/>
       <c r="T26" s="21"/>
-      <c r="U26" s="64">
+      <c r="U26" s="52">
         <v>8489</v>
       </c>
       <c r="V26" s="32"/>
@@ -2273,7 +2266,7 @@
       <c r="AO26" s="4"/>
       <c r="AP26" s="5"/>
     </row>
-    <row r="27" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="32"/>
       <c r="C27" s="7"/>
@@ -2317,7 +2310,7 @@
       <c r="AO27" s="4"/>
       <c r="AP27" s="5"/>
     </row>
-    <row r="28" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="32"/>
       <c r="C28" s="7"/>
@@ -2361,7 +2354,7 @@
       <c r="AO28" s="4"/>
       <c r="AP28" s="5"/>
     </row>
-    <row r="29" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="32"/>
       <c r="C29" s="6"/>
@@ -2405,7 +2398,7 @@
       <c r="AO29" s="27"/>
       <c r="AP29" s="5"/>
     </row>
-    <row r="30" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="32"/>
       <c r="C30" s="6"/>
@@ -2449,7 +2442,7 @@
       <c r="AO30" s="27"/>
       <c r="AP30" s="5"/>
     </row>
-    <row r="31" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="32"/>
       <c r="C31" s="6"/>
@@ -2493,7 +2486,7 @@
       <c r="AO31" s="27"/>
       <c r="AP31" s="5"/>
     </row>
-    <row r="32" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="32"/>
       <c r="C32" s="6"/>
@@ -2537,11 +2530,11 @@
       <c r="AO32" s="27"/>
       <c r="AP32" s="5"/>
     </row>
-    <row r="33" spans="1:44" s="1" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:44" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="32"/>
       <c r="C33" s="6"/>
-      <c r="D33" s="57">
+      <c r="D33" s="47">
         <v>5921</v>
       </c>
       <c r="E33" s="6"/>
@@ -2551,13 +2544,13 @@
       <c r="I33" s="6"/>
       <c r="J33" s="32"/>
       <c r="K33" s="6"/>
-      <c r="L33" s="57">
+      <c r="L33" s="47">
         <v>5913</v>
       </c>
       <c r="M33" s="6"/>
       <c r="N33" s="32"/>
       <c r="O33" s="4"/>
-      <c r="P33" s="57">
+      <c r="P33" s="47">
         <v>5946</v>
       </c>
       <c r="Q33" s="4"/>
@@ -2567,13 +2560,13 @@
       <c r="U33" s="4"/>
       <c r="V33" s="32"/>
       <c r="W33" s="4"/>
-      <c r="X33" s="57">
+      <c r="X33" s="47">
         <v>5927</v>
       </c>
       <c r="Y33" s="4"/>
       <c r="Z33" s="32"/>
       <c r="AA33" s="4"/>
-      <c r="AB33" s="57">
+      <c r="AB33" s="47">
         <v>5356</v>
       </c>
       <c r="AC33" s="27"/>
@@ -2587,27 +2580,27 @@
       <c r="AK33" s="27"/>
       <c r="AL33" s="32"/>
       <c r="AM33" s="27"/>
-      <c r="AN33" s="57">
+      <c r="AN33" s="47">
         <v>3592</v>
       </c>
       <c r="AO33" s="27"/>
       <c r="AP33" s="5"/>
     </row>
     <row r="38" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="AR38" s="62">
+      <c r="AR38" s="50">
         <v>5909</v>
       </c>
     </row>
     <row r="44" spans="1:44" ht="23" x14ac:dyDescent="0.25">
-      <c r="R44" s="61" t="s">
+      <c r="R44" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="S44" s="61"/>
-      <c r="T44" s="61"/>
-      <c r="U44" s="61"/>
+      <c r="S44" s="55"/>
+      <c r="T44" s="55"/>
+      <c r="U44" s="55"/>
     </row>
     <row r="45" spans="1:44" x14ac:dyDescent="0.2">
-      <c r="AG45" s="63">
+      <c r="AG45" s="51">
         <v>8486</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data update and daily log
</commit_message>
<xml_diff>
--- a/planning/greenhouse_design/greenhousedesign.xlsx
+++ b/planning/greenhouse_design/greenhousedesign.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/planning/greenhouse_design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22712A46-0E81-D64D-A5AF-658715A53F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8762E3D-F427-1D4C-B3C2-570F6C44C3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{D6621B14-A242-0E4C-80F5-D7CC9E637369}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -608,6 +608,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="180" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -955,8 +958,8 @@
   </sheetPr>
   <dimension ref="A1:BB45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="93" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1268,7 +1271,7 @@
       <c r="A5" s="4"/>
       <c r="B5" s="32"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="41"/>
+      <c r="D5" s="64"/>
       <c r="E5" s="4"/>
       <c r="F5" s="32"/>
       <c r="G5" s="4"/>
@@ -2490,7 +2493,7 @@
       <c r="A32" s="6"/>
       <c r="B32" s="32"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="46"/>
+      <c r="D32" s="64"/>
       <c r="E32" s="6"/>
       <c r="F32" s="32"/>
       <c r="G32" s="6"/>

</xml_diff>